<commit_message>
Finished Validate and Add Appointments modules
</commit_message>
<xml_diff>
--- a/Documents/Appointments.xlsx
+++ b/Documents/Appointments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FACULTATE\Licenta\HealthClinicSolution\HealthClinic\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29829E79-780C-40C9-854D-8BA7523FEFA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D9101CC-913B-4597-9C50-711A33231F4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>First name</t>
   </si>
@@ -33,70 +33,13 @@
     <t>Last name</t>
   </si>
   <si>
-    <t>ana</t>
-  </si>
-  <si>
-    <t>georgescu</t>
-  </si>
-  <si>
-    <t>ilie</t>
-  </si>
-  <si>
-    <t>popa</t>
-  </si>
-  <si>
-    <t>rares</t>
-  </si>
-  <si>
-    <t>matei</t>
-  </si>
-  <si>
-    <t>ion</t>
-  </si>
-  <si>
-    <t>ionescu</t>
-  </si>
-  <si>
     <t>Phone number</t>
   </si>
   <si>
-    <t>Appointment date</t>
-  </si>
-  <si>
     <t>Doctor name</t>
   </si>
   <si>
-    <t>0765123457</t>
-  </si>
-  <si>
-    <t>0725433269</t>
-  </si>
-  <si>
-    <t>0771295667</t>
-  </si>
-  <si>
-    <t>0721224547</t>
-  </si>
-  <si>
-    <t>0722896689</t>
-  </si>
-  <si>
-    <t>Milea Denis</t>
-  </si>
-  <si>
-    <t>Chitu George</t>
-  </si>
-  <si>
-    <t>Popa Cristinel</t>
-  </si>
-  <si>
-    <t>Pantelimon Irina</t>
-  </si>
-  <si>
-    <t>mateescu</t>
-  </si>
-  <si>
-    <t>george</t>
+    <t>Appointment dAte</t>
   </si>
 </sst>
 </file>
@@ -132,10 +75,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,20 +357,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -439,98 +373,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
         <v>3</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="2">
-        <v>44658.4375</v>
-      </c>
-      <c r="E2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="2">
-        <v>44658.5</v>
-      </c>
-      <c r="E3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="2">
-        <v>44658.645833333336</v>
-      </c>
-      <c r="E4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="2">
-        <v>44659.333333333336</v>
-      </c>
-      <c r="E5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="2">
-        <v>44659.354166666664</v>
-      </c>
-      <c r="E6" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added e-mail sending library; send e-mail for insufficient stock
</commit_message>
<xml_diff>
--- a/Documents/Appointments.xlsx
+++ b/Documents/Appointments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FACULTATE\Licenta\HealthClinicSolution\HealthClinic\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9ACE0A4-6397-4508-9F85-5B4724CBE229}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E16282D9-A6D6-40A8-81D5-F932214B8BEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5985" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>First name</t>
   </si>
@@ -40,21 +40,6 @@
   </si>
   <si>
     <t>Appointment dAte</t>
-  </si>
-  <si>
-    <t>ana</t>
-  </si>
-  <si>
-    <t>ionescu</t>
-  </si>
-  <si>
-    <t>075555555</t>
-  </si>
-  <si>
-    <t>28.05.2022 13:00</t>
-  </si>
-  <si>
-    <t>Marian Popa</t>
   </si>
 </sst>
 </file>
@@ -372,10 +357,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A2" sqref="A2:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -397,23 +382,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added German language + Bug fixing
</commit_message>
<xml_diff>
--- a/Documents/Appointments.xlsx
+++ b/Documents/Appointments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FACULTATE\Licenta\HealthClinicSolution\HealthClinic\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A66D6CEC-B11D-44F3-8ECC-3849FF6FB3E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7480CEB-478C-4567-A93B-F96FC231E4E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5985" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Appointments" sheetId="1" r:id="rId1"/>
@@ -360,7 +360,7 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E3"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>